<commit_message>
Release v2.1: Added right-click rating feature
</commit_message>
<xml_diff>
--- a/data/air_quality_city_list.xlsx
+++ b/data/air_quality_city_list.xlsx
@@ -711,12 +711,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>辽宁</t>
+          <t>四川</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>葫芦岛</t>
+          <t>资阳</t>
         </is>
       </c>
     </row>
@@ -726,12 +726,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>四川</t>
+          <t>辽宁</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>资阳</t>
+          <t>葫芦岛</t>
         </is>
       </c>
     </row>
@@ -741,12 +741,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>四川</t>
+          <t>吉林</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>广安</t>
+          <t>长春</t>
         </is>
       </c>
     </row>
@@ -756,12 +756,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>吉林</t>
+          <t>四川</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>长春</t>
+          <t>广安</t>
         </is>
       </c>
     </row>
@@ -876,12 +876,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>山东</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>滨州</t>
+          <t>洛阳</t>
         </is>
       </c>
     </row>
@@ -891,12 +891,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>山东</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>洛阳</t>
+          <t>滨州</t>
         </is>
       </c>
     </row>
@@ -1056,12 +1056,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>河北</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>新乡</t>
+          <t>邯郸</t>
         </is>
       </c>
     </row>
@@ -1071,12 +1071,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>山东</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>安阳</t>
+          <t>潍坊</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>四川</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>南充</t>
+          <t>新乡</t>
         </is>
       </c>
     </row>
@@ -1101,12 +1101,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>河北</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>邯郸</t>
+          <t>安阳</t>
         </is>
       </c>
     </row>
@@ -1116,12 +1116,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>山东</t>
+          <t>四川</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>潍坊</t>
+          <t>南充</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>山东</t>
+          <t>山西</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>临沂</t>
+          <t>太原</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>山西</t>
+          <t>山东</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>太原</t>
+          <t>临沂</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>济南</t>
+          <t>德州</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>德州</t>
+          <t>济南</t>
         </is>
       </c>
     </row>
@@ -1296,12 +1296,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>山东</t>
+          <t>安徽</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>枣庄</t>
+          <t>亳州</t>
         </is>
       </c>
     </row>
@@ -1311,12 +1311,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>安徽</t>
+          <t>山东</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>亳州</t>
+          <t>日照</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>日照</t>
+          <t>枣庄</t>
         </is>
       </c>
     </row>
@@ -1371,12 +1371,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>陕西</t>
+          <t>安徽</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>宝鸡</t>
+          <t>宿州</t>
         </is>
       </c>
     </row>
@@ -1386,12 +1386,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>安徽</t>
+          <t>陕西</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>宿州</t>
+          <t>宝鸡</t>
         </is>
       </c>
     </row>
@@ -1446,12 +1446,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>山西</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>吕梁</t>
+          <t>连云港</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>四川</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>雅安</t>
+          <t>南阳</t>
         </is>
       </c>
     </row>
@@ -1476,12 +1476,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>山西</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>郑州</t>
+          <t>吕梁</t>
         </is>
       </c>
     </row>
@@ -1491,12 +1491,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>山东</t>
+          <t>四川</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>济宁</t>
+          <t>雅安</t>
         </is>
       </c>
     </row>
@@ -1506,12 +1506,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>连云港</t>
+          <t>郑州</t>
         </is>
       </c>
     </row>
@@ -1521,12 +1521,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>山东</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>南阳</t>
+          <t>济宁</t>
         </is>
       </c>
     </row>
@@ -1596,12 +1596,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>宿迁</t>
+          <t>许昌</t>
         </is>
       </c>
     </row>
@@ -1611,12 +1611,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>许昌</t>
+          <t>宿迁</t>
         </is>
       </c>
     </row>
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>四川</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>泸州</t>
+          <t>开封</t>
         </is>
       </c>
     </row>
@@ -1641,12 +1641,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>四川</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>平顶山</t>
+          <t>泸州</t>
         </is>
       </c>
     </row>
@@ -1656,12 +1656,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>徐州</t>
+          <t>平顶山</t>
         </is>
       </c>
     </row>
@@ -1671,12 +1671,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>驻马店</t>
+          <t>徐州</t>
         </is>
       </c>
     </row>
@@ -1686,12 +1686,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>武汉</t>
+          <t>驻马店</t>
         </is>
       </c>
     </row>
@@ -1701,12 +1701,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>开封</t>
+          <t>武汉</t>
         </is>
       </c>
     </row>
@@ -1761,12 +1761,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>山西</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>朔州</t>
+          <t>孝感</t>
         </is>
       </c>
     </row>
@@ -1776,12 +1776,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>孝感</t>
+          <t>漯河</t>
         </is>
       </c>
     </row>
@@ -1791,12 +1791,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>山西</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>漯河</t>
+          <t>朔州</t>
         </is>
       </c>
     </row>
@@ -1851,12 +1851,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>浙江</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>随州</t>
+          <t>湖州</t>
         </is>
       </c>
     </row>
@@ -1866,12 +1866,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>淮安</t>
+          <t>随州</t>
         </is>
       </c>
     </row>
@@ -1881,12 +1881,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>四川</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>遂宁</t>
+          <t>淮安</t>
         </is>
       </c>
     </row>
@@ -1896,12 +1896,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>四川</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>襄阳</t>
+          <t>遂宁</t>
         </is>
       </c>
     </row>
@@ -1911,12 +1911,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>宁夏</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>银川</t>
+          <t>襄阳</t>
         </is>
       </c>
     </row>
@@ -1926,12 +1926,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>浙江</t>
+          <t>宁夏</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>湖州</t>
+          <t>银川</t>
         </is>
       </c>
     </row>
@@ -1956,12 +1956,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>湖南</t>
+          <t>安徽</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>益阳</t>
+          <t>淮北</t>
         </is>
       </c>
     </row>
@@ -1971,12 +1971,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>安徽</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>淮北</t>
+          <t>常州</t>
         </is>
       </c>
     </row>
@@ -1986,12 +1986,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>湖南</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>常州</t>
+          <t>益阳</t>
         </is>
       </c>
     </row>
@@ -2046,12 +2046,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>青海</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>西宁</t>
+          <t>盐城</t>
         </is>
       </c>
     </row>
@@ -2061,12 +2061,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>安徽</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>盐城</t>
+          <t>六安</t>
         </is>
       </c>
     </row>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>六安</t>
+          <t>蚌埠</t>
         </is>
       </c>
     </row>
@@ -2091,12 +2091,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>安徽</t>
+          <t>湖南</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>蚌埠</t>
+          <t>岳阳</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>湖南</t>
+          <t>青海</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>岳阳</t>
+          <t>西宁</t>
         </is>
       </c>
     </row>
@@ -2166,12 +2166,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>山西</t>
+          <t>广东</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>大同</t>
+          <t>广州</t>
         </is>
       </c>
     </row>
@@ -2181,12 +2181,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>广东</t>
+          <t>新疆</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>广州</t>
+          <t>乌鲁木齐</t>
         </is>
       </c>
     </row>
@@ -2196,12 +2196,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>新疆</t>
+          <t>贵州</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>乌鲁木齐</t>
+          <t>贵阳</t>
         </is>
       </c>
     </row>
@@ -2211,12 +2211,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>贵州</t>
+          <t>山西</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>贵阳</t>
+          <t>大同</t>
         </is>
       </c>
     </row>
@@ -2226,12 +2226,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>安徽</t>
+          <t>江西</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>铜陵</t>
+          <t>新余</t>
         </is>
       </c>
     </row>
@@ -2241,12 +2241,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>江西</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>新余</t>
+          <t>荆门</t>
         </is>
       </c>
     </row>
@@ -2256,12 +2256,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>安徽</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>荆门</t>
+          <t>铜陵</t>
         </is>
       </c>
     </row>
@@ -2271,12 +2271,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>鄂州</t>
+          <t>扬州</t>
         </is>
       </c>
     </row>
@@ -2286,12 +2286,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>扬州</t>
+          <t>鄂州</t>
         </is>
       </c>
     </row>
@@ -2301,12 +2301,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>湖南</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>无锡</t>
+          <t>常德</t>
         </is>
       </c>
     </row>
@@ -2316,12 +2316,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>荆州</t>
+          <t>无锡</t>
         </is>
       </c>
     </row>
@@ -2331,12 +2331,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>南通</t>
+          <t>荆州</t>
         </is>
       </c>
     </row>
@@ -2346,12 +2346,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>湖南</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>常德</t>
+          <t>南通</t>
         </is>
       </c>
     </row>
@@ -2361,12 +2361,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>湖南</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>长沙</t>
+          <t>咸宁</t>
         </is>
       </c>
     </row>
@@ -2376,12 +2376,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>湖南</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>咸宁</t>
+          <t>长沙</t>
         </is>
       </c>
     </row>
@@ -2421,12 +2421,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>辽宁</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>黄冈</t>
+          <t>大连</t>
         </is>
       </c>
     </row>
@@ -2436,12 +2436,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>辽宁</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>大连</t>
+          <t>黄冈</t>
         </is>
       </c>
     </row>
@@ -2466,12 +2466,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>浙江</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>绍兴</t>
+          <t>黄石</t>
         </is>
       </c>
     </row>
@@ -2481,12 +2481,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>福建</t>
+          <t>浙江</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>厦门</t>
+          <t>绍兴</t>
         </is>
       </c>
     </row>
@@ -2496,12 +2496,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>福建</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>黄石</t>
+          <t>厦门</t>
         </is>
       </c>
     </row>
@@ -2616,12 +2616,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>湖南</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>湘潭</t>
+          <t>南京</t>
         </is>
       </c>
     </row>
@@ -2631,12 +2631,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>江苏</t>
+          <t>湖南</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>南京</t>
+          <t>湘潭</t>
         </is>
       </c>
     </row>
@@ -2811,12 +2811,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>广西</t>
+          <t>浙江</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>南宁</t>
+          <t>台州</t>
         </is>
       </c>
     </row>
@@ -2826,12 +2826,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>浙江</t>
+          <t>广西</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>台州</t>
+          <t>南宁</t>
         </is>
       </c>
     </row>

</xml_diff>